<commit_message>
colored text not added
</commit_message>
<xml_diff>
--- a/spec/ooxl/resources/test.xlsx
+++ b/spec/ooxl/resources/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\salsify\gems\ooxml_excel\spec\ooxl\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\salsify\gems\ooxl\spec\ooxl\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
     <definedName name="named_range">Sheet2!$A$1:$A$2</definedName>
     <definedName name="range">Sheet2!$A$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Sample Title</t>
   </si>
@@ -57,13 +57,27 @@
   </si>
   <si>
     <t>Range Value 2</t>
+  </si>
+  <si>
+    <r>
+      <t>Range Valu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -76,6 +90,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -547,7 +567,7 @@
   <dimension ref="A1:AMK2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -557,7 +577,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2">
         <v>2</v>

</xml_diff>

<commit_message>
support for fetching cell range values without specifying row indexes
</commit_message>
<xml_diff>
--- a/spec/ooxl/resources/test.xlsx
+++ b/spec/ooxl/resources/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="named_range">Sheet2!$A$1:$A$2</definedName>
     <definedName name="range">Sheet2!$A$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -537,6 +537,9 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12345</v>
+      </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -572,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
last column and stream row
</commit_message>
<xml_diff>
--- a/spec/ooxl/resources/test.xlsx
+++ b/spec/ooxl/resources/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\salsify\gems\ooxl\spec\ooxl\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\salsify\others\gems\ooxl\spec\ooxl\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -486,14 +486,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="8.5703125"/>
     <col min="3" max="3" width="0" hidden="1"/>
-    <col min="4" max="1025" width="8.5703125"/>
+    <col min="4" max="1024" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>